<commit_message>
almost complete with TSCA2019-inspired clean ups
</commit_message>
<xml_diff>
--- a/TSCA2019/tables_manually_reviewed/TSCA2019_culture_folders_to_review_2023-03-02_afc.xlsx
+++ b/TSCA2019/tables_manually_reviewed/TSCA2019_culture_folders_to_review_2023-03-02_afc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acarpe01\Documents\local_repos\pre-process_mea_acute_for_tcpl\TSCA2019\tables_manually_reviewed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2837559B-3894-4BAC-A1FC-53587930C15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52FE5D2-10B7-45AF-8784-1F57FECD9BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="-15480" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22980" yWindow="-16365" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TSCA cultures" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="116">
   <si>
     <t>culture_folders</t>
   </si>
@@ -257,9 +257,6 @@
     <t>72-8208 - get clarification on impact of recording while offset was running.</t>
   </si>
   <si>
-    <t>Will see if plate 72-8209 looks that much different than the other replicates (given the baseline decline, 20-24 min of rest might matter?)</t>
-  </si>
-  <si>
     <t>confirm that this means that the doses should be switched in the calculations files, then do that</t>
   </si>
   <si>
@@ -312,12 +309,6 @@
   </si>
   <si>
     <t>need lab followup org</t>
-  </si>
-  <si>
-    <t>See convo with Tim 3/7/23 - MEA activity should not be affected, but there could be interference in the LDH or AB. Do follow up analysis). Still need to check up on sinking stuff.</t>
-  </si>
-  <si>
-    <t>See convo with Tim 3/7/23 - MEA activity should not be affected, but there could be interference in the LDH or AB. Do follow up analysis). Still need to check up on sinking stuff, still need to do follow up on combining recording (though that might be analysis)</t>
   </si>
   <si>
     <t>Theresa/seline/someone created a spliced version for some endpoints. Will consider if I trust that, and if consistent with other spliced files.</t>
@@ -348,17 +339,10 @@
     <t>check for potential interference in LDH or AB for this compound; view situation re sinking</t>
   </si>
   <si>
-    <t xml:space="preserve">Regarding 40 min Treated Start time: Plate 72-8208 "hit stop began recording while offset was running"
-Regarding 40 min Treated Start time: Plate 72-8209 "recording had stopped. Thought I had forgot to start it. Started it again then realized mistake. Actual start time was 2:18 pm" </t>
-  </si>
-  <si>
     <t>Regarding Pate 72-8209: (actual start time is only 4 min late. I doubt this is a deal-breaker, but I've made a note to analyze all cases where analysis start or duration is off)</t>
   </si>
   <si>
     <t>Theresa/Seline</t>
-  </si>
-  <si>
-    <t>Seline explained that after hitting start, Axion runs an “offset” as a preliminary calibration step. I guess they usually hit record after this offset has completed. However, the offset only takes about 10 seconds. Therefore, for a 40 minute recording, the effect of including a 10-sec offset should probably not affect the parameter values too much.</t>
   </si>
   <si>
     <t>Compare plate 75-5802 to the other 2 plates for the LDH values to confirm if okay to normalize by experiment date (despite the slighlty lower volume of substrate)</t>
@@ -381,9 +365,6 @@
 As for whether the data is still usable overall, Seline said that if Theresa continued with the assay, she probably thought is was still usable… but wouldn’t hurt to check the values.</t>
   </si>
   <si>
-    <t>check if plate 75-8114 looks okay despite tipping</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plate 1 should be slipped 180 degrees, as was the case for G11. (i.e., well A8 should be well F1). No reorientation has been implemented in the raw or Calculations file.
 Seline confirmed that the raw data files for G20 and G21. She probably just forgot to copy &amp; paste the updated values into the Calculations file. This made her question whether she should go back and manually check every other culture… I said I would do that with R.
 </t>
@@ -396,6 +377,25 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>check if plate 75-8114 looks okay despite tipping. Well quality already set to 0 for wells G3 and H3, but check if other wells appear usable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See convo with Tim 3/7/23 - MEA activity should not be affected, but there could be interference in the LDH or AB. Do follow up analysis). Still need to check up on whether we care about solution sinking to bottom of well. </t>
+  </si>
+  <si>
+    <t>See convo with Tim 3/7/23 - MEA activity should not be affected, but there could be interference in the LDH or AB. Do follow up analysis). Still need to check up on whether we care about solution sinking to bottom of well, still need to do follow up on combining recording (though that might be analysis)</t>
+  </si>
+  <si>
+    <t>Regarding Plate 72-8208, Seline explained that after hitting start, Axion runs an “offset” as a preliminary calibration step. I guess they usually hit record after this offset has completed. However, the offset only takes about 10 seconds. Therefore, for a 40 minute recording, the effect of including a 10-sec offset should probably not affect the parameter values too much.</t>
+  </si>
+  <si>
+    <t>Regarding 40 min Treated Start time: Plate 72-8208 "hit stop began recording while offset was running"
+Regarding 40 min Treated Start time: Plate 72-8209 "recording had stopped. Thought I had forgot to start it. Started it again then realized mistake. Actual start time was 2:18 pm" (should have been 2:04 pm, so the recording was started 34 minutes after treatment was added rather than the usual 20 minutes)</t>
+  </si>
+  <si>
+    <t>Will see if plate 72-8209 looks that much different than the other replicates (given the decline in activity over time, an extra 14 mintues of 'rest' after treatment addition might matter?)</t>
   </si>
 </sst>
 </file>
@@ -744,9 +744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,28 +776,28 @@
         <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>57</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -837,7 +837,7 @@
         <v>44987</v>
       </c>
       <c r="E3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -869,7 +869,7 @@
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
         <v>64</v>
@@ -881,10 +881,10 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K4" t="s">
         <v>89</v>
-      </c>
-      <c r="K4" t="s">
-        <v>90</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -936,7 +936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="144" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -944,19 +944,19 @@
         <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D7" s="2">
         <v>44987</v>
       </c>
       <c r="E7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F7" t="s">
         <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -965,10 +965,10 @@
         <v>0</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="K7" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="L7">
         <v>1</v>
@@ -1005,19 +1005,19 @@
         <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D9" s="2">
         <v>44988</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -1026,10 +1026,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="K9" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1072,10 +1072,10 @@
         <v>44988</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="F11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
         <v>48</v>
@@ -1087,13 +1087,13 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="331.2" x14ac:dyDescent="0.3">
@@ -1104,19 +1104,19 @@
         <v>44</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D12" s="2">
         <v>44988</v>
       </c>
       <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
         <v>76</v>
       </c>
-      <c r="F12" t="s">
-        <v>77</v>
-      </c>
       <c r="G12" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -1125,10 +1125,10 @@
         <v>0</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1223,7 +1223,7 @@
         <v>44988</v>
       </c>
       <c r="F16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G16" t="s">
         <v>64</v>
@@ -1235,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
+        <v>88</v>
+      </c>
+      <c r="K16" t="s">
         <v>89</v>
-      </c>
-      <c r="K16" t="s">
-        <v>90</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -1258,22 +1258,22 @@
         <v>44988</v>
       </c>
       <c r="E17" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" t="s">
         <v>78</v>
       </c>
-      <c r="F17" t="s">
-        <v>79</v>
-      </c>
       <c r="G17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
         <v>104</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
-        <v>109</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -1339,13 +1339,13 @@
         <v>44988</v>
       </c>
       <c r="E20" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" t="s">
         <v>80</v>
       </c>
-      <c r="F20" t="s">
-        <v>81</v>
-      </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -1354,10 +1354,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K20" t="s">
         <v>110</v>
-      </c>
-      <c r="K20" t="s">
-        <v>111</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -1383,7 +1383,7 @@
         <v>61</v>
       </c>
       <c r="G21" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -1392,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="K21" t="s">
         <v>58</v>
@@ -1453,10 +1453,10 @@
         <v>1</v>
       </c>
       <c r="J23" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="K23" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -1496,13 +1496,13 @@
         <v>44</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D25" s="2">
         <v>44988</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F25" t="s">
         <v>63</v>
@@ -1517,10 +1517,10 @@
         <v>1</v>
       </c>
       <c r="J25" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="K25" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L25">
         <v>1</v>
@@ -1716,10 +1716,10 @@
         <v>1</v>
       </c>
       <c r="J33" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="K33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L33">
         <v>1</v>

</xml_diff>